<commit_message>
Anpassungen aus Sprintreview eingfügt
Aspekte der Teamkommunikation in die Prozess-FMEA aufgenommen.
</commit_message>
<xml_diff>
--- a/FMEA/FMEA_Process.xlsx
+++ b/FMEA/FMEA_Process.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="FMEA_Prozess" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="87">
   <si>
     <t>Erzeugnis</t>
   </si>
@@ -136,9 +137,6 @@
     <t>Keine "Mischung"</t>
   </si>
   <si>
-    <t>Projektmitglieder definieren</t>
-  </si>
-  <si>
     <t>Nur unerfahrene Projektmitglieder gewählt</t>
   </si>
   <si>
@@ -257,12 +255,33 @@
   </si>
   <si>
     <t>Versuchen alle möglichen use cases abzudecken</t>
+  </si>
+  <si>
+    <t>Projektarbeit</t>
+  </si>
+  <si>
+    <t>Teamkommunikation</t>
+  </si>
+  <si>
+    <t>Mangelhafter Informationsaustausch</t>
+  </si>
+  <si>
+    <t>Schlechte Abstimmung im Team</t>
+  </si>
+  <si>
+    <t>Technische Probleme in der Kommunikation</t>
+  </si>
+  <si>
+    <t>Erprobung der Kommunikationswege vor der Nutzung</t>
+  </si>
+  <si>
+    <t>Regelmäßige Abstimmungstermine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -446,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -524,18 +543,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -545,97 +651,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -656,7 +678,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -731,23 +753,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -783,23 +788,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -976,24 +964,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="63.42578125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.85546875" style="9" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="11"/>
-    <col min="10" max="10" width="83.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.86328125" customWidth="1"/>
+    <col min="2" max="2" width="37.40625" customWidth="1"/>
+    <col min="3" max="3" width="63.40625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="37.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.86328125" style="9" customWidth="1"/>
+    <col min="6" max="9" width="9.1328125" style="11"/>
+    <col min="10" max="10" width="83.40625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1006,66 +994,66 @@
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="38" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="30" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A2" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="48">
-        <v>6</v>
-      </c>
-      <c r="G2" s="48">
+      <c r="F2" s="40">
+        <v>6</v>
+      </c>
+      <c r="G2" s="40">
         <v>2</v>
       </c>
-      <c r="H2" s="48">
+      <c r="H2" s="40">
         <v>2</v>
       </c>
       <c r="I2" s="18">
-        <f t="shared" ref="I2:I21" si="0">F2*G2*H2</f>
+        <f t="shared" ref="I2:I23" si="0">F2*G2*H2</f>
         <v>24</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.65">
+      <c r="A3" s="65"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="44" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="10">
@@ -1077,24 +1065,24 @@
       <c r="H3" s="10">
         <v>2</v>
       </c>
-      <c r="I3" s="44">
+      <c r="I3" s="36">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.65">
+      <c r="A4" s="65"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="45" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="10">
@@ -1106,19 +1094,19 @@
       <c r="H4" s="10">
         <v>2</v>
       </c>
-      <c r="I4" s="44"/>
+      <c r="I4" s="36"/>
       <c r="J4" s="22" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="41" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="28.5" x14ac:dyDescent="0.65">
+      <c r="A5" s="65"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="44" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="10">
@@ -1130,62 +1118,62 @@
       <c r="H5" s="10">
         <v>6</v>
       </c>
-      <c r="I5" s="44">
+      <c r="I5" s="36">
         <f t="shared" si="0"/>
         <v>108</v>
       </c>
       <c r="J5" s="22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="28.75" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A6" s="65"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="42">
+        <v>6</v>
+      </c>
+      <c r="G6" s="42">
+        <v>4</v>
+      </c>
+      <c r="H6" s="42">
+        <v>2</v>
+      </c>
+      <c r="I6" s="19">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="J6" s="23" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="54" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="50">
-        <v>6</v>
-      </c>
-      <c r="G6" s="50">
-        <v>4</v>
-      </c>
-      <c r="H6" s="50">
-        <v>2</v>
-      </c>
-      <c r="I6" s="19">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="J6" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="28" t="s">
+    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A7" s="65"/>
+      <c r="B7" s="57" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="55" t="s">
+      <c r="E7" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="48">
+      <c r="F7" s="40">
         <v>8</v>
       </c>
-      <c r="G7" s="48">
+      <c r="G7" s="40">
         <v>3</v>
       </c>
-      <c r="H7" s="48">
+      <c r="H7" s="40">
         <v>2</v>
       </c>
       <c r="I7" s="18">
@@ -1193,19 +1181,19 @@
         <v>48</v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.65">
+      <c r="A8" s="65"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="52" t="s">
+      <c r="E8" s="44" t="s">
         <v>32</v>
       </c>
       <c r="F8" s="10">
@@ -1217,22 +1205,22 @@
       <c r="H8" s="10">
         <v>5</v>
       </c>
-      <c r="I8" s="44">
+      <c r="I8" s="36">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="38"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A9" s="65"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="64"/>
       <c r="D9" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="54" t="s">
+      <c r="E9" s="46" t="s">
         <v>34</v>
       </c>
       <c r="F9" s="10">
@@ -1249,292 +1237,290 @@
         <v>75</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A10" s="65"/>
+      <c r="B10" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="62" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>38</v>
       </c>
       <c r="E10" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="50">
+        <v>8</v>
+      </c>
+      <c r="G10" s="40">
+        <v>5</v>
+      </c>
+      <c r="H10" s="51">
+        <v>2</v>
+      </c>
+      <c r="I10" s="49">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A11" s="65"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="58">
-        <v>8</v>
-      </c>
-      <c r="G10" s="48">
-        <v>5</v>
-      </c>
-      <c r="H10" s="59">
-        <v>2</v>
-      </c>
-      <c r="I10" s="57">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="J10" s="23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="60">
+      <c r="F11" s="52">
         <v>8</v>
       </c>
       <c r="G11" s="10">
         <v>5</v>
       </c>
-      <c r="H11" s="61">
+      <c r="H11" s="53">
         <v>2</v>
       </c>
-      <c r="I11" s="57">
+      <c r="I11" s="49">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="J11" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A12" s="65"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="52">
+        <v>9</v>
+      </c>
+      <c r="G12" s="39">
+        <v>8</v>
+      </c>
+      <c r="H12" s="53">
+        <v>1</v>
+      </c>
+      <c r="I12" s="49">
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="16" t="s">
+      <c r="J12" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A13" s="65"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="52">
+        <v>9</v>
+      </c>
+      <c r="G13" s="39">
+        <v>5</v>
+      </c>
+      <c r="H13" s="53">
+        <v>6</v>
+      </c>
+      <c r="I13" s="49">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
+      <c r="J13" s="22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A14" s="65"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D14" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="54">
+        <v>8</v>
+      </c>
+      <c r="G14" s="42">
+        <v>2</v>
+      </c>
+      <c r="H14" s="55">
+        <v>2</v>
+      </c>
+      <c r="I14" s="49">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A15" s="65"/>
+      <c r="B15" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="62">
+      <c r="D15" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="10">
         <v>8</v>
       </c>
-      <c r="G12" s="50">
+      <c r="G15" s="10">
+        <v>6</v>
+      </c>
+      <c r="H15" s="10">
+        <v>4</v>
+      </c>
+      <c r="I15" s="18">
+        <f t="shared" si="0"/>
+        <v>192</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A16" s="65"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="10">
+        <v>8</v>
+      </c>
+      <c r="G16" s="10">
         <v>2</v>
       </c>
-      <c r="H12" s="63">
+      <c r="H16" s="10">
         <v>2</v>
       </c>
-      <c r="I12" s="57">
+      <c r="I16" s="18">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="J12" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="27"/>
-      <c r="B13" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="55" t="s">
+      <c r="J16" s="21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A17" s="65"/>
+      <c r="B17" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="50">
+        <v>6</v>
+      </c>
+      <c r="G17" s="40">
+        <v>6</v>
+      </c>
+      <c r="H17" s="51">
+        <v>2</v>
+      </c>
+      <c r="I17" s="41">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A18" s="65"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="52">
+        <v>6</v>
+      </c>
+      <c r="G18" s="10">
+        <v>6</v>
+      </c>
+      <c r="H18" s="53">
+        <v>6</v>
+      </c>
+      <c r="I18" s="41">
+        <f t="shared" si="0"/>
+        <v>216</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="28.75" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A19" s="65"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="10">
-        <v>8</v>
-      </c>
-      <c r="G13" s="10">
-        <v>6</v>
-      </c>
-      <c r="H13" s="10">
-        <v>4</v>
-      </c>
-      <c r="I13" s="18">
-        <f t="shared" si="0"/>
-        <v>192</v>
-      </c>
-      <c r="J13" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="56" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="10">
-        <v>8</v>
-      </c>
-      <c r="G14" s="10">
+      <c r="D19" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="52">
+        <v>6</v>
+      </c>
+      <c r="G19" s="10">
+        <v>6</v>
+      </c>
+      <c r="H19" s="53">
         <v>2</v>
       </c>
-      <c r="H14" s="10">
-        <v>2</v>
-      </c>
-      <c r="I14" s="18">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="J14" s="21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="58">
-        <v>6</v>
-      </c>
-      <c r="G15" s="48">
-        <v>6</v>
-      </c>
-      <c r="H15" s="59">
-        <v>2</v>
-      </c>
-      <c r="I15" s="49">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="60">
-        <v>6</v>
-      </c>
-      <c r="G16" s="10">
-        <v>6</v>
-      </c>
-      <c r="H16" s="61">
-        <v>6</v>
-      </c>
-      <c r="I16" s="49">
-        <f t="shared" si="0"/>
-        <v>216</v>
-      </c>
-      <c r="J16" s="25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="60">
-        <v>6</v>
-      </c>
-      <c r="G17" s="10">
-        <v>6</v>
-      </c>
-      <c r="H17" s="61">
-        <v>2</v>
-      </c>
-      <c r="I17" s="49">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="J17" s="25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="60">
-        <v>6</v>
-      </c>
-      <c r="G18" s="10">
-        <v>6</v>
-      </c>
-      <c r="H18" s="61">
-        <v>6</v>
-      </c>
-      <c r="I18" s="49">
-        <f t="shared" si="0"/>
-        <v>216</v>
-      </c>
-      <c r="J18" s="25" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="60">
-        <v>6</v>
-      </c>
-      <c r="G19" s="10">
-        <v>6</v>
-      </c>
-      <c r="H19" s="61">
-        <v>2</v>
-      </c>
-      <c r="I19" s="49">
+      <c r="I19" s="41">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
@@ -1542,99 +1528,169 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27"/>
-      <c r="B20" s="29"/>
+    <row r="20" spans="1:10" ht="28.75" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A20" s="65"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="39" t="s">
+      <c r="D20" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="52">
+        <v>6</v>
+      </c>
+      <c r="G20" s="10">
+        <v>6</v>
+      </c>
+      <c r="H20" s="53">
+        <v>6</v>
+      </c>
+      <c r="I20" s="41">
+        <f t="shared" si="0"/>
+        <v>216</v>
+      </c>
+      <c r="J20" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A21" s="65"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="52">
+        <v>6</v>
+      </c>
+      <c r="G21" s="10">
+        <v>6</v>
+      </c>
+      <c r="H21" s="53">
+        <v>2</v>
+      </c>
+      <c r="I21" s="41">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="J21" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A22" s="65"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="52">
+        <v>6</v>
+      </c>
+      <c r="G22" s="10">
+        <v>6</v>
+      </c>
+      <c r="H22" s="53">
+        <v>6</v>
+      </c>
+      <c r="I22" s="41">
+        <f t="shared" si="0"/>
+        <v>216</v>
+      </c>
+      <c r="J22" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A23" s="65"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="E23" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="60">
-        <v>6</v>
-      </c>
-      <c r="G20" s="10">
-        <v>6</v>
-      </c>
-      <c r="H20" s="61">
-        <v>6</v>
-      </c>
-      <c r="I20" s="49">
-        <f t="shared" si="0"/>
-        <v>216</v>
-      </c>
-      <c r="J20" s="25" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="27"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="40" t="s">
+      <c r="F23" s="54">
+        <v>9</v>
+      </c>
+      <c r="G23" s="42">
+        <v>6</v>
+      </c>
+      <c r="H23" s="55">
+        <v>6</v>
+      </c>
+      <c r="I23" s="56">
+        <f t="shared" si="0"/>
+        <v>324</v>
+      </c>
+      <c r="J23" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="62">
-        <v>9</v>
-      </c>
-      <c r="G21" s="50">
-        <v>6</v>
-      </c>
-      <c r="H21" s="63">
-        <v>6</v>
-      </c>
-      <c r="I21" s="64">
-        <f t="shared" si="0"/>
-        <v>324</v>
-      </c>
-      <c r="J21" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.65">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="10"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.65">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.65">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B21"/>
+  <mergeCells count="12">
+    <mergeCell ref="A2:A23"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B23"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B10:B14"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A2:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>